<commit_message>
completed account-service impl and mart-cart-service impl
</commit_message>
<xml_diff>
--- a/Design&Spec/PathList.xlsx
+++ b/Design&Spec/PathList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSD-assignment\Design&amp;Spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C33356-C233-4613-AC51-E51DF067105D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECFBFCC-13CD-4D17-9920-D9DBFBAF5C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
   <si>
     <t>Working</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -165,6 +165,10 @@
   </si>
   <si>
     <t>Project Path:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected to be completed on 5/17/2020</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -545,9 +549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DE9D6E-AA71-486D-91E4-7F44082E4F93}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -558,10 +564,11 @@
     <col min="6" max="6" width="9" style="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="34.875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -569,8 +576,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -578,8 +585,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -587,8 +594,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -596,13 +603,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -628,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -654,7 +661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -674,13 +681,16 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -706,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -726,13 +736,16 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -757,8 +770,11 @@
       <c r="H15" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -783,8 +799,11 @@
       <c r="H16" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -809,8 +828,11 @@
       <c r="H17" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -835,8 +857,11 @@
       <c r="H18" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -860,6 +885,9 @@
       </c>
       <c r="H19" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -880,5 +908,6 @@
     <hyperlink ref="B11" r:id="rId13" xr:uid="{9BFAF0AB-0A0B-4F9E-8F2F-AAAB7D3F702C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>